<commit_message>
puse la version de mi tarea de Semana 3 de Google Drive
</commit_message>
<xml_diff>
--- a/Semana 4/COSTO DE REPORTOS EMISIÓN DE BONOS U OBLIGACIONES - ACCIONES.xlsx
+++ b/Semana 4/COSTO DE REPORTOS EMISIÓN DE BONOS U OBLIGACIONES - ACCIONES.xlsx
@@ -5,17 +5,18 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\cid_c\OneDrive\Documentos\UNITEC\MAESTRIA UNITEC\FINANZAS GERENCIALES - FINANZAS SÁBADOS 26022022\SEMANA 4\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\megam\Unitec\Master en Finanzas\masterFinanzasFinanzasGerenciales\Semana 4\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{FB64E777-7108-490F-A5EA-BE37782F4644}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{195CC107-4F5D-4FF5-ADDD-A04D5853E59D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{6194F04A-3D98-4C32-A125-94F82D0CE0F9}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="14020" activeTab="2" xr2:uid="{6194F04A-3D98-4C32-A125-94F82D0CE0F9}"/>
   </bookViews>
   <sheets>
     <sheet name="REPORTO PRIVADO" sheetId="1" r:id="rId1"/>
     <sheet name="TASA DE INDIFERENCIA" sheetId="3" r:id="rId2"/>
     <sheet name="EMISIÓN BONOS ACCIONES" sheetId="4" r:id="rId3"/>
+    <sheet name="Sheet1" sheetId="5" r:id="rId4"/>
   </sheets>
   <calcPr calcId="191029" concurrentCalc="0"/>
   <extLst>
@@ -674,64 +675,64 @@
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="4" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="4" fontId="4" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="9" fontId="3" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="10" fontId="3" fillId="0" borderId="5" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="10" fontId="3" fillId="0" borderId="6" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="10" fontId="3" fillId="0" borderId="7" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="4" fontId="4" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="10" fontId="3" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="justify" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="justify" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="9" fontId="3" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="10" fontId="3" fillId="0" borderId="5" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="10" fontId="3" fillId="0" borderId="6" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="10" fontId="3" fillId="0" borderId="7" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="4" fontId="4" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="4" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="4" fontId="4" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Porcentaje" xfId="1" builtinId="5"/>
+    <cellStyle name="Percent" xfId="1" builtinId="5"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -747,7 +748,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema de Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -1045,25 +1046,25 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7DE10229-30A6-4FF6-99DF-93C043230550}">
   <dimension ref="A2:D19"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="10.90625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="2" max="2" width="36.5703125" customWidth="1"/>
-    <col min="3" max="3" width="5.85546875" customWidth="1"/>
-    <col min="4" max="4" width="12.85546875" customWidth="1"/>
-    <col min="5" max="5" width="3.42578125" customWidth="1"/>
-    <col min="6" max="6" width="11.28515625" customWidth="1"/>
-    <col min="7" max="7" width="4.28515625" customWidth="1"/>
-    <col min="8" max="8" width="11.5703125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="3.42578125" customWidth="1"/>
-    <col min="10" max="10" width="11.85546875" customWidth="1"/>
-    <col min="11" max="11" width="4.140625" customWidth="1"/>
-    <col min="13" max="13" width="2.85546875" customWidth="1"/>
-    <col min="14" max="14" width="9.7109375" customWidth="1"/>
+    <col min="2" max="2" width="36.54296875" customWidth="1"/>
+    <col min="3" max="3" width="5.81640625" customWidth="1"/>
+    <col min="4" max="4" width="12.81640625" customWidth="1"/>
+    <col min="5" max="5" width="3.453125" customWidth="1"/>
+    <col min="6" max="6" width="11.26953125" customWidth="1"/>
+    <col min="7" max="7" width="4.26953125" customWidth="1"/>
+    <col min="8" max="8" width="11.54296875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="3.453125" customWidth="1"/>
+    <col min="10" max="10" width="11.81640625" customWidth="1"/>
+    <col min="11" max="11" width="4.1796875" customWidth="1"/>
+    <col min="13" max="13" width="2.81640625" customWidth="1"/>
+    <col min="14" max="14" width="9.7265625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:4" ht="18" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" ht="18" x14ac:dyDescent="0.4">
       <c r="A2" s="46" t="s">
         <v>59</v>
       </c>
@@ -1071,7 +1072,7 @@
       <c r="C2" s="46"/>
       <c r="D2" s="46"/>
     </row>
-    <row r="4" spans="1:4" ht="18" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4" ht="18" x14ac:dyDescent="0.4">
       <c r="A4" s="46" t="s">
         <v>26</v>
       </c>
@@ -1079,7 +1080,7 @@
       <c r="C4" s="46"/>
       <c r="D4" s="46"/>
     </row>
-    <row r="6" spans="1:4" ht="18.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:4" ht="18.5" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A6" s="47" t="s">
         <v>21</v>
       </c>
@@ -1093,7 +1094,7 @@
         <v>360</v>
       </c>
     </row>
-    <row r="7" spans="1:4" ht="18" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:4" ht="18" x14ac:dyDescent="0.4">
       <c r="A7" s="47"/>
       <c r="B7" s="10" t="s">
         <v>23</v>
@@ -1103,7 +1104,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="10" spans="1:4" ht="20.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:4" ht="20.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A10" s="47" t="s">
         <v>21</v>
       </c>
@@ -1117,7 +1118,7 @@
         <v>360</v>
       </c>
     </row>
-    <row r="11" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A11" s="47"/>
       <c r="B11" s="14">
         <v>2500000</v>
@@ -1127,8 +1128,8 @@
         <v>8</v>
       </c>
     </row>
-    <row r="13" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="14" spans="1:4" ht="24.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.4"/>
+    <row r="14" spans="1:4" ht="24.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A14" s="11" t="s">
         <v>21</v>
       </c>
@@ -1144,10 +1145,10 @@
         <v>45</v>
       </c>
     </row>
-    <row r="15" spans="1:4" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:4" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A15" s="13"/>
     </row>
-    <row r="16" spans="1:4" ht="25.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:4" ht="25.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A16" s="11" t="s">
         <v>21</v>
       </c>
@@ -1156,8 +1157,8 @@
         <v>0.16000002000000235</v>
       </c>
     </row>
-    <row r="18" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="19" spans="1:2" ht="21.75" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="18" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.4"/>
+    <row r="19" spans="1:2" ht="21.5" thickBot="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A19" s="44" t="s">
         <v>60</v>
       </c>
@@ -1185,12 +1186,12 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="10.90625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="59.5703125" customWidth="1"/>
+    <col min="1" max="1" width="59.54296875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:6" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:6" ht="18.5" x14ac:dyDescent="0.45">
       <c r="A2" s="51" t="s">
         <v>27</v>
       </c>
@@ -1200,7 +1201,7 @@
       <c r="E2" s="51"/>
       <c r="F2" s="51"/>
     </row>
-    <row r="3" spans="1:6" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:6" ht="18.5" x14ac:dyDescent="0.45">
       <c r="A3" s="51" t="s">
         <v>28</v>
       </c>
@@ -1210,8 +1211,8 @@
       <c r="E3" s="51"/>
       <c r="F3" s="51"/>
     </row>
-    <row r="4" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="5" spans="1:6" ht="61.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.4"/>
+    <row r="5" spans="1:6" ht="61.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A5" s="52" t="s">
         <v>29</v>
       </c>
@@ -1221,9 +1222,9 @@
       <c r="E5" s="53"/>
       <c r="F5" s="54"/>
     </row>
-    <row r="6" spans="1:6" ht="12" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="7" spans="1:6" ht="10.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="8" spans="1:6" ht="47.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:6" ht="12" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="7" spans="1:6" ht="10.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.4"/>
+    <row r="8" spans="1:6" ht="47.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A8" s="52" t="s">
         <v>30</v>
       </c>
@@ -1233,7 +1234,7 @@
       <c r="E8" s="53"/>
       <c r="F8" s="54"/>
     </row>
-    <row r="10" spans="1:6" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:6" ht="18.5" x14ac:dyDescent="0.45">
       <c r="A10" s="24" t="s">
         <v>31</v>
       </c>
@@ -1243,7 +1244,7 @@
       <c r="C10" s="24"/>
       <c r="D10" s="24"/>
     </row>
-    <row r="11" spans="1:6" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:6" ht="18.5" x14ac:dyDescent="0.45">
       <c r="A11" s="24" t="s">
         <v>32</v>
       </c>
@@ -1253,7 +1254,7 @@
       <c r="C11" s="24"/>
       <c r="D11" s="24"/>
     </row>
-    <row r="12" spans="1:6" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:6" ht="18.5" x14ac:dyDescent="0.45">
       <c r="A12" s="24" t="s">
         <v>33</v>
       </c>
@@ -1261,7 +1262,7 @@
       <c r="C12" s="24"/>
       <c r="D12" s="24"/>
     </row>
-    <row r="13" spans="1:6" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:6" ht="18.5" x14ac:dyDescent="0.45">
       <c r="A13" s="25">
         <v>1</v>
       </c>
@@ -1273,7 +1274,7 @@
       </c>
       <c r="D13" s="24"/>
     </row>
-    <row r="14" spans="1:6" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:6" ht="18.5" x14ac:dyDescent="0.45">
       <c r="A14" s="25">
         <v>2</v>
       </c>
@@ -1285,7 +1286,7 @@
       </c>
       <c r="D14" s="24"/>
     </row>
-    <row r="15" spans="1:6" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:6" ht="18.5" x14ac:dyDescent="0.45">
       <c r="A15" s="25">
         <v>3</v>
       </c>
@@ -1297,7 +1298,7 @@
       </c>
       <c r="D15" s="24"/>
     </row>
-    <row r="16" spans="1:6" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:6" ht="18.5" x14ac:dyDescent="0.45">
       <c r="A16" s="25">
         <v>4</v>
       </c>
@@ -1309,7 +1310,7 @@
       </c>
       <c r="D16" s="24"/>
     </row>
-    <row r="17" spans="1:6" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:6" ht="18.5" x14ac:dyDescent="0.45">
       <c r="A17" s="25">
         <v>5</v>
       </c>
@@ -1321,7 +1322,7 @@
       </c>
       <c r="D17" s="24"/>
     </row>
-    <row r="18" spans="1:6" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:6" ht="18.5" x14ac:dyDescent="0.45">
       <c r="A18" s="25">
         <v>6</v>
       </c>
@@ -1333,13 +1334,13 @@
       </c>
       <c r="D18" s="24"/>
     </row>
-    <row r="19" spans="1:6" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:6" ht="12.75" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A19" s="24"/>
       <c r="B19" s="24"/>
       <c r="C19" s="24"/>
       <c r="D19" s="24"/>
     </row>
-    <row r="20" spans="1:6" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:6" ht="18.5" x14ac:dyDescent="0.45">
       <c r="A20" s="24" t="s">
         <v>35</v>
       </c>
@@ -1347,7 +1348,7 @@
       <c r="C20" s="24"/>
       <c r="D20" s="24"/>
     </row>
-    <row r="22" spans="1:6" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:6" ht="18.5" x14ac:dyDescent="0.45">
       <c r="A22" s="55" t="s">
         <v>36</v>
       </c>
@@ -1357,15 +1358,15 @@
       <c r="E22" s="55"/>
       <c r="F22" s="55"/>
     </row>
-    <row r="23" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="24" spans="1:6" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.4"/>
+    <row r="24" spans="1:6" ht="19" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A24" s="29" t="s">
         <v>37</v>
       </c>
       <c r="B24" s="30"/>
     </row>
-    <row r="26" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="27" spans="1:6" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.4"/>
+    <row r="27" spans="1:6" ht="18.5" x14ac:dyDescent="0.45">
       <c r="A27" s="31" t="s">
         <v>38</v>
       </c>
@@ -1375,7 +1376,7 @@
       <c r="C27" s="32"/>
       <c r="D27" s="33"/>
     </row>
-    <row r="28" spans="1:6" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:6" ht="18.5" x14ac:dyDescent="0.45">
       <c r="A28" s="34" t="s">
         <v>34</v>
       </c>
@@ -1385,7 +1386,7 @@
       <c r="C28" s="24"/>
       <c r="D28" s="35"/>
     </row>
-    <row r="29" spans="1:6" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:6" ht="19" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A29" s="36" t="s">
         <v>41</v>
       </c>
@@ -1395,13 +1396,13 @@
       <c r="C29" s="37"/>
       <c r="D29" s="38"/>
     </row>
-    <row r="30" spans="1:6" ht="12" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:6" ht="12" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A30" s="39"/>
     </row>
-    <row r="31" spans="1:6" ht="9.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:6" ht="9.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A31" s="39"/>
     </row>
-    <row r="32" spans="1:6" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:6" ht="18.5" x14ac:dyDescent="0.45">
       <c r="A32" s="55" t="s">
         <v>43</v>
       </c>
@@ -1411,10 +1412,10 @@
       <c r="E32" s="55"/>
       <c r="F32" s="55"/>
     </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A33" s="39"/>
     </row>
-    <row r="34" spans="1:4" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:4" ht="18.5" x14ac:dyDescent="0.45">
       <c r="A34" s="40" t="s">
         <v>44</v>
       </c>
@@ -1424,7 +1425,7 @@
       <c r="C34" s="24"/>
       <c r="D34" s="24"/>
     </row>
-    <row r="35" spans="1:4" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:4" ht="18.5" x14ac:dyDescent="0.45">
       <c r="A35" s="40" t="s">
         <v>44</v>
       </c>
@@ -1435,13 +1436,13 @@
       <c r="C35" s="24"/>
       <c r="D35" s="24"/>
     </row>
-    <row r="36" spans="1:4" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:4" ht="18.5" x14ac:dyDescent="0.45">
       <c r="A36" s="25"/>
       <c r="B36" s="24"/>
       <c r="C36" s="24"/>
       <c r="D36" s="24"/>
     </row>
-    <row r="37" spans="1:4" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:4" ht="18.5" x14ac:dyDescent="0.45">
       <c r="A37" s="40" t="s">
         <v>46</v>
       </c>
@@ -1451,7 +1452,7 @@
       <c r="C37" s="24"/>
       <c r="D37" s="24"/>
     </row>
-    <row r="38" spans="1:4" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:4" ht="18.5" x14ac:dyDescent="0.45">
       <c r="A38" s="40" t="s">
         <v>46</v>
       </c>
@@ -1462,13 +1463,13 @@
       <c r="C38" s="24"/>
       <c r="D38" s="24"/>
     </row>
-    <row r="39" spans="1:4" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:4" ht="18.5" x14ac:dyDescent="0.45">
       <c r="A39" s="25"/>
       <c r="B39" s="24"/>
       <c r="C39" s="24"/>
       <c r="D39" s="24"/>
     </row>
-    <row r="40" spans="1:4" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:4" ht="18.5" x14ac:dyDescent="0.45">
       <c r="A40" s="40" t="s">
         <v>48</v>
       </c>
@@ -1478,7 +1479,7 @@
       <c r="C40" s="24"/>
       <c r="D40" s="24"/>
     </row>
-    <row r="41" spans="1:4" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:4" ht="18.5" x14ac:dyDescent="0.45">
       <c r="A41" s="40" t="s">
         <v>48</v>
       </c>
@@ -1489,13 +1490,13 @@
       <c r="C41" s="24"/>
       <c r="D41" s="24"/>
     </row>
-    <row r="42" spans="1:4" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:4" ht="18.5" x14ac:dyDescent="0.45">
       <c r="A42" s="25"/>
       <c r="B42" s="24"/>
       <c r="C42" s="24"/>
       <c r="D42" s="24"/>
     </row>
-    <row r="43" spans="1:4" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:4" ht="18.5" x14ac:dyDescent="0.45">
       <c r="A43" s="40" t="s">
         <v>50</v>
       </c>
@@ -1505,7 +1506,7 @@
       <c r="C43" s="24"/>
       <c r="D43" s="24"/>
     </row>
-    <row r="44" spans="1:4" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:4" ht="18.5" x14ac:dyDescent="0.45">
       <c r="A44" s="40" t="s">
         <v>50</v>
       </c>
@@ -1516,13 +1517,13 @@
       <c r="C44" s="24"/>
       <c r="D44" s="24"/>
     </row>
-    <row r="45" spans="1:4" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:4" ht="18.5" x14ac:dyDescent="0.45">
       <c r="A45" s="25"/>
       <c r="B45" s="24"/>
       <c r="C45" s="24"/>
       <c r="D45" s="24"/>
     </row>
-    <row r="46" spans="1:4" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:4" ht="18.5" x14ac:dyDescent="0.45">
       <c r="A46" s="40" t="s">
         <v>52</v>
       </c>
@@ -1532,7 +1533,7 @@
       <c r="C46" s="24"/>
       <c r="D46" s="24"/>
     </row>
-    <row r="47" spans="1:4" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:4" ht="18.5" x14ac:dyDescent="0.45">
       <c r="A47" s="40" t="s">
         <v>52</v>
       </c>
@@ -1543,13 +1544,13 @@
       <c r="C47" s="24"/>
       <c r="D47" s="24"/>
     </row>
-    <row r="48" spans="1:4" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:4" ht="18.5" x14ac:dyDescent="0.45">
       <c r="A48" s="25"/>
       <c r="B48" s="24"/>
       <c r="C48" s="24"/>
       <c r="D48" s="24"/>
     </row>
-    <row r="49" spans="1:6" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:6" ht="18.5" x14ac:dyDescent="0.45">
       <c r="A49" s="40" t="s">
         <v>54</v>
       </c>
@@ -1559,7 +1560,7 @@
       <c r="C49" s="24"/>
       <c r="D49" s="24"/>
     </row>
-    <row r="50" spans="1:6" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:6" ht="18.5" x14ac:dyDescent="0.45">
       <c r="A50" s="40" t="s">
         <v>54</v>
       </c>
@@ -1570,17 +1571,17 @@
       <c r="C50" s="24"/>
       <c r="D50" s="24"/>
     </row>
-    <row r="51" spans="1:6" ht="11.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="52" spans="1:6" ht="6" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="53" spans="1:6" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:6" ht="11.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="52" spans="1:6" ht="6" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="53" spans="1:6" ht="18.5" x14ac:dyDescent="0.45">
       <c r="A53" s="42" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="54" spans="1:6" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="54" spans="1:6" ht="19" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A54" s="42"/>
     </row>
-    <row r="55" spans="1:6" ht="41.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:6" ht="41.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A55" s="48" t="s">
         <v>57</v>
       </c>
@@ -1590,9 +1591,9 @@
       <c r="E55" s="49"/>
       <c r="F55" s="50"/>
     </row>
-    <row r="56" spans="1:6" ht="10.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="57" spans="1:6" ht="9" customHeight="1" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="58" spans="1:6" ht="39.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:6" ht="10.5" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="57" spans="1:6" ht="9" customHeight="1" thickBot="1" x14ac:dyDescent="0.4"/>
+    <row r="58" spans="1:6" ht="39.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A58" s="48" t="s">
         <v>58</v>
       </c>
@@ -1602,7 +1603,7 @@
       <c r="E58" s="49"/>
       <c r="F58" s="50"/>
     </row>
-    <row r="59" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A59" s="43"/>
       <c r="B59" s="43"/>
       <c r="C59" s="43"/>
@@ -1628,25 +1629,27 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{998B2EA8-8A31-456B-9775-CC19B59BC6F4}">
   <dimension ref="A2:N36"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="A14" workbookViewId="0">
+      <selection activeCell="G38" sqref="G38"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="10.90625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="2" max="2" width="36.5703125" customWidth="1"/>
-    <col min="3" max="3" width="5.85546875" customWidth="1"/>
-    <col min="4" max="4" width="12.85546875" customWidth="1"/>
-    <col min="5" max="5" width="3.42578125" customWidth="1"/>
-    <col min="6" max="6" width="11.28515625" customWidth="1"/>
-    <col min="7" max="7" width="4.28515625" customWidth="1"/>
-    <col min="8" max="8" width="11.5703125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="3.42578125" customWidth="1"/>
-    <col min="10" max="10" width="11.85546875" customWidth="1"/>
-    <col min="11" max="11" width="4.140625" customWidth="1"/>
-    <col min="13" max="13" width="2.85546875" customWidth="1"/>
-    <col min="14" max="14" width="9.7109375" customWidth="1"/>
+    <col min="2" max="2" width="36.54296875" customWidth="1"/>
+    <col min="3" max="3" width="5.81640625" customWidth="1"/>
+    <col min="4" max="4" width="12.81640625" customWidth="1"/>
+    <col min="5" max="5" width="3.453125" customWidth="1"/>
+    <col min="6" max="6" width="11.26953125" customWidth="1"/>
+    <col min="7" max="7" width="4.26953125" customWidth="1"/>
+    <col min="8" max="8" width="11.54296875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="3.453125" customWidth="1"/>
+    <col min="10" max="10" width="11.81640625" customWidth="1"/>
+    <col min="11" max="11" width="4.1796875" customWidth="1"/>
+    <col min="13" max="13" width="2.81640625" customWidth="1"/>
+    <col min="14" max="14" width="9.7265625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:14" ht="18" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:14" ht="18" x14ac:dyDescent="0.4">
       <c r="A2" s="46" t="s">
         <v>0</v>
       </c>
@@ -1660,7 +1663,7 @@
       <c r="I2" s="23"/>
       <c r="J2" s="23"/>
     </row>
-    <row r="3" spans="1:14" ht="18" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:14" ht="18" x14ac:dyDescent="0.4">
       <c r="A3" s="21"/>
       <c r="B3" s="21"/>
       <c r="C3" s="21"/>
@@ -1672,7 +1675,7 @@
       <c r="I3" s="21"/>
       <c r="J3" s="21"/>
     </row>
-    <row r="4" spans="1:14" ht="18" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:14" ht="18" x14ac:dyDescent="0.4">
       <c r="A4" s="47" t="s">
         <v>1</v>
       </c>
@@ -1696,10 +1699,10 @@
       <c r="I4" s="21"/>
       <c r="J4" s="21"/>
     </row>
-    <row r="5" spans="1:14" ht="18.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:14" ht="18.5" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A5" s="47"/>
-      <c r="B5" s="72"/>
-      <c r="C5" s="72"/>
+      <c r="B5" s="56"/>
+      <c r="C5" s="56"/>
       <c r="D5" s="20" t="s">
         <v>10</v>
       </c>
@@ -1710,13 +1713,13 @@
       <c r="I5" s="21"/>
       <c r="J5" s="21"/>
     </row>
-    <row r="6" spans="1:14" ht="18.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:14" ht="18.5" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A6" s="47"/>
-      <c r="B6" s="73" t="s">
+      <c r="B6" s="57" t="s">
         <v>11</v>
       </c>
-      <c r="C6" s="73"/>
-      <c r="D6" s="73"/>
+      <c r="C6" s="57"/>
+      <c r="D6" s="57"/>
       <c r="E6" s="47"/>
       <c r="F6" s="47"/>
       <c r="G6" s="21"/>
@@ -1724,13 +1727,13 @@
       <c r="I6" s="21"/>
       <c r="J6" s="21"/>
     </row>
-    <row r="7" spans="1:14" ht="18" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:14" ht="18" x14ac:dyDescent="0.4">
       <c r="A7" s="47"/>
-      <c r="B7" s="61">
+      <c r="B7" s="58">
         <v>2</v>
       </c>
-      <c r="C7" s="61"/>
-      <c r="D7" s="61"/>
+      <c r="C7" s="58"/>
+      <c r="D7" s="58"/>
       <c r="E7" s="47"/>
       <c r="F7" s="47"/>
       <c r="G7" s="21"/>
@@ -1738,7 +1741,7 @@
       <c r="I7" s="21"/>
       <c r="J7" s="21"/>
     </row>
-    <row r="8" spans="1:14" ht="18" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:14" ht="18" x14ac:dyDescent="0.4">
       <c r="A8" s="19"/>
       <c r="B8" s="21"/>
       <c r="C8" s="21"/>
@@ -1750,7 +1753,7 @@
       <c r="I8" s="21"/>
       <c r="J8" s="21"/>
     </row>
-    <row r="9" spans="1:14" ht="18.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:14" ht="18.5" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A9" s="21"/>
       <c r="B9" s="21"/>
       <c r="C9" s="21"/>
@@ -1762,11 +1765,11 @@
       <c r="I9" s="21"/>
       <c r="J9" s="21"/>
     </row>
-    <row r="10" spans="1:14" ht="18.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:14" ht="18" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A10" s="47" t="s">
         <v>1</v>
       </c>
-      <c r="B10" s="70">
+      <c r="B10" s="59">
         <v>21.25</v>
       </c>
       <c r="C10" s="2" t="s">
@@ -1781,97 +1784,97 @@
       <c r="F10" s="3">
         <v>200</v>
       </c>
-      <c r="G10" s="62" t="s">
+      <c r="G10" s="61" t="s">
         <v>4</v>
       </c>
-      <c r="H10" s="70">
+      <c r="H10" s="59">
         <f>B10+(D10-F10)/D11</f>
         <v>37.916666666666671</v>
       </c>
-      <c r="I10" s="62" t="s">
+      <c r="I10" s="61" t="s">
         <v>4</v>
       </c>
-      <c r="J10" s="56">
+      <c r="J10" s="69">
         <f>H10/H12</f>
         <v>0.16851851851851854</v>
       </c>
-      <c r="K10" s="62" t="s">
+      <c r="K10" s="61" t="s">
         <v>12</v>
       </c>
-      <c r="L10" s="63">
+      <c r="L10" s="62">
         <f>1-0.42</f>
         <v>0.58000000000000007</v>
       </c>
-      <c r="M10" s="62" t="s">
+      <c r="M10" s="61" t="s">
         <v>4</v>
       </c>
-      <c r="N10" s="64">
+      <c r="N10" s="63">
         <f>J10*L10</f>
         <v>9.7740740740740767E-2</v>
       </c>
     </row>
-    <row r="11" spans="1:14" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:14" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A11" s="47"/>
-      <c r="B11" s="71"/>
+      <c r="B11" s="60"/>
       <c r="C11" s="5"/>
-      <c r="D11" s="67">
+      <c r="D11" s="66">
         <v>3</v>
       </c>
-      <c r="E11" s="67"/>
-      <c r="F11" s="67"/>
-      <c r="G11" s="62"/>
-      <c r="H11" s="71"/>
-      <c r="I11" s="62"/>
-      <c r="J11" s="56"/>
-      <c r="K11" s="62"/>
-      <c r="L11" s="63"/>
-      <c r="M11" s="62"/>
-      <c r="N11" s="65"/>
-    </row>
-    <row r="12" spans="1:14" ht="18.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="E11" s="66"/>
+      <c r="F11" s="66"/>
+      <c r="G11" s="61"/>
+      <c r="H11" s="60"/>
+      <c r="I11" s="61"/>
+      <c r="J11" s="69"/>
+      <c r="K11" s="61"/>
+      <c r="L11" s="62"/>
+      <c r="M11" s="61"/>
+      <c r="N11" s="64"/>
+    </row>
+    <row r="12" spans="1:14" ht="18.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A12" s="47"/>
-      <c r="B12" s="68">
+      <c r="B12" s="67">
         <v>250</v>
       </c>
-      <c r="C12" s="68"/>
-      <c r="D12" s="68"/>
+      <c r="C12" s="67"/>
+      <c r="D12" s="67"/>
       <c r="E12" s="22" t="s">
         <v>2</v>
       </c>
       <c r="F12" s="6">
         <v>200</v>
       </c>
-      <c r="G12" s="62"/>
+      <c r="G12" s="61"/>
       <c r="H12" s="7">
         <f>(B12+F12)/B13</f>
         <v>225</v>
       </c>
-      <c r="I12" s="62"/>
-      <c r="J12" s="56"/>
-      <c r="K12" s="62"/>
-      <c r="L12" s="63"/>
-      <c r="M12" s="62"/>
-      <c r="N12" s="65"/>
-    </row>
-    <row r="13" spans="1:14" ht="18.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="I12" s="61"/>
+      <c r="J12" s="69"/>
+      <c r="K12" s="61"/>
+      <c r="L12" s="62"/>
+      <c r="M12" s="61"/>
+      <c r="N12" s="64"/>
+    </row>
+    <row r="13" spans="1:14" ht="18" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A13" s="47"/>
-      <c r="B13" s="69">
+      <c r="B13" s="68">
         <v>2</v>
       </c>
-      <c r="C13" s="69"/>
-      <c r="D13" s="69"/>
-      <c r="E13" s="69"/>
-      <c r="F13" s="69"/>
+      <c r="C13" s="68"/>
+      <c r="D13" s="68"/>
+      <c r="E13" s="68"/>
+      <c r="F13" s="68"/>
       <c r="G13" s="8"/>
       <c r="H13" s="1"/>
       <c r="I13" s="1"/>
-      <c r="J13" s="56"/>
-      <c r="K13" s="62"/>
-      <c r="L13" s="63"/>
-      <c r="M13" s="62"/>
-      <c r="N13" s="66"/>
-    </row>
-    <row r="14" spans="1:14" ht="18" x14ac:dyDescent="0.25">
+      <c r="J13" s="69"/>
+      <c r="K13" s="61"/>
+      <c r="L13" s="62"/>
+      <c r="M13" s="61"/>
+      <c r="N13" s="65"/>
+    </row>
+    <row r="14" spans="1:14" ht="18" x14ac:dyDescent="0.35">
       <c r="A14" s="19"/>
       <c r="B14" s="2"/>
       <c r="C14" s="2"/>
@@ -1883,73 +1886,73 @@
       <c r="I14" s="1"/>
       <c r="J14" s="18"/>
     </row>
-    <row r="16" spans="1:14" ht="41.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="60" t="s">
+    <row r="16" spans="1:14" ht="41.25" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A16" s="70" t="s">
         <v>6</v>
       </c>
-      <c r="B16" s="60"/>
-      <c r="C16" s="60"/>
-      <c r="D16" s="60"/>
-      <c r="E16" s="60"/>
-      <c r="F16" s="60"/>
-      <c r="G16" s="60"/>
-      <c r="H16" s="60"/>
-      <c r="I16" s="60"/>
-      <c r="J16" s="60"/>
-    </row>
-    <row r="18" spans="1:10" ht="77.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="60" t="s">
+      <c r="B16" s="70"/>
+      <c r="C16" s="70"/>
+      <c r="D16" s="70"/>
+      <c r="E16" s="70"/>
+      <c r="F16" s="70"/>
+      <c r="G16" s="70"/>
+      <c r="H16" s="70"/>
+      <c r="I16" s="70"/>
+      <c r="J16" s="70"/>
+    </row>
+    <row r="18" spans="1:10" ht="77.25" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A18" s="70" t="s">
         <v>7</v>
       </c>
-      <c r="B18" s="60"/>
-      <c r="C18" s="60"/>
-      <c r="D18" s="60"/>
-      <c r="E18" s="60"/>
-      <c r="F18" s="60"/>
-      <c r="G18" s="60"/>
-      <c r="H18" s="60"/>
-      <c r="I18" s="60"/>
-      <c r="J18" s="60"/>
-    </row>
-    <row r="20" spans="1:10" ht="72" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="60" t="s">
+      <c r="B18" s="70"/>
+      <c r="C18" s="70"/>
+      <c r="D18" s="70"/>
+      <c r="E18" s="70"/>
+      <c r="F18" s="70"/>
+      <c r="G18" s="70"/>
+      <c r="H18" s="70"/>
+      <c r="I18" s="70"/>
+      <c r="J18" s="70"/>
+    </row>
+    <row r="20" spans="1:10" ht="72" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A20" s="70" t="s">
         <v>5</v>
       </c>
-      <c r="B20" s="60"/>
-      <c r="C20" s="60"/>
-      <c r="D20" s="60"/>
-      <c r="E20" s="60"/>
-      <c r="F20" s="60"/>
-      <c r="G20" s="60"/>
-      <c r="H20" s="60"/>
-      <c r="I20" s="60"/>
-      <c r="J20" s="60"/>
-    </row>
-    <row r="23" spans="1:10" ht="18" x14ac:dyDescent="0.25">
-      <c r="A23" s="57" t="s">
+      <c r="B20" s="70"/>
+      <c r="C20" s="70"/>
+      <c r="D20" s="70"/>
+      <c r="E20" s="70"/>
+      <c r="F20" s="70"/>
+      <c r="G20" s="70"/>
+      <c r="H20" s="70"/>
+      <c r="I20" s="70"/>
+      <c r="J20" s="70"/>
+    </row>
+    <row r="23" spans="1:10" ht="18" x14ac:dyDescent="0.4">
+      <c r="A23" s="71" t="s">
         <v>14</v>
       </c>
-      <c r="B23" s="57"/>
-      <c r="C23" s="57"/>
-      <c r="D23" s="57"/>
-      <c r="E23" s="57"/>
-      <c r="F23" s="57"/>
-      <c r="G23" s="57"/>
-      <c r="H23" s="57"/>
-      <c r="I23" s="57"/>
-      <c r="J23" s="57"/>
-    </row>
-    <row r="25" spans="1:10" ht="18.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B23" s="71"/>
+      <c r="C23" s="71"/>
+      <c r="D23" s="71"/>
+      <c r="E23" s="71"/>
+      <c r="F23" s="71"/>
+      <c r="G23" s="71"/>
+      <c r="H23" s="71"/>
+      <c r="I23" s="71"/>
+      <c r="J23" s="71"/>
+    </row>
+    <row r="25" spans="1:10" ht="18.5" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A25" s="47" t="s">
         <v>15</v>
       </c>
-      <c r="B25" s="59" t="s">
+      <c r="B25" s="72" t="s">
         <v>16</v>
       </c>
-      <c r="C25" s="59"/>
-      <c r="D25" s="59"/>
-      <c r="E25" s="59"/>
-      <c r="F25" s="59"/>
+      <c r="C25" s="72"/>
+      <c r="D25" s="72"/>
+      <c r="E25" s="72"/>
+      <c r="F25" s="72"/>
       <c r="G25" s="47" t="s">
         <v>2</v>
       </c>
@@ -1958,20 +1961,20 @@
       </c>
       <c r="I25" s="9"/>
     </row>
-    <row r="26" spans="1:10" ht="18" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:10" ht="18" x14ac:dyDescent="0.4">
       <c r="A26" s="47"/>
-      <c r="B26" s="61" t="s">
+      <c r="B26" s="58" t="s">
         <v>20</v>
       </c>
-      <c r="C26" s="61"/>
-      <c r="D26" s="61"/>
-      <c r="E26" s="61"/>
-      <c r="F26" s="61"/>
+      <c r="C26" s="58"/>
+      <c r="D26" s="58"/>
+      <c r="E26" s="58"/>
+      <c r="F26" s="58"/>
       <c r="G26" s="47"/>
       <c r="H26" s="47"/>
       <c r="I26" s="9"/>
     </row>
-    <row r="27" spans="1:10" ht="18" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:10" ht="17.5" x14ac:dyDescent="0.35">
       <c r="A27" s="1"/>
       <c r="B27" s="1"/>
       <c r="C27" s="1"/>
@@ -1981,19 +1984,19 @@
       <c r="G27" s="1"/>
       <c r="H27" s="1"/>
     </row>
-    <row r="28" spans="1:10" ht="18" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:10" ht="18" x14ac:dyDescent="0.4">
       <c r="A28" s="1"/>
-      <c r="B28" s="57" t="s">
+      <c r="B28" s="71" t="s">
         <v>18</v>
       </c>
-      <c r="C28" s="57"/>
-      <c r="D28" s="57"/>
-      <c r="E28" s="57"/>
-      <c r="F28" s="57"/>
-      <c r="G28" s="57"/>
-      <c r="H28" s="57"/>
-    </row>
-    <row r="29" spans="1:10" ht="18" x14ac:dyDescent="0.25">
+      <c r="C28" s="71"/>
+      <c r="D28" s="71"/>
+      <c r="E28" s="71"/>
+      <c r="F28" s="71"/>
+      <c r="G28" s="71"/>
+      <c r="H28" s="71"/>
+    </row>
+    <row r="29" spans="1:10" ht="17.5" x14ac:dyDescent="0.35">
       <c r="A29" s="1"/>
       <c r="B29" s="1"/>
       <c r="C29" s="1"/>
@@ -2003,7 +2006,7 @@
       <c r="G29" s="1"/>
       <c r="H29" s="1"/>
     </row>
-    <row r="30" spans="1:10" ht="18.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:10" ht="18.5" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A30" s="47" t="s">
         <v>15</v>
       </c>
@@ -2013,7 +2016,7 @@
       <c r="C30" s="21" t="s">
         <v>2</v>
       </c>
-      <c r="D30" s="58" t="s">
+      <c r="D30" s="73" t="s">
         <v>17</v>
       </c>
       <c r="E30" s="1"/>
@@ -2021,19 +2024,19 @@
       <c r="G30" s="1"/>
       <c r="H30" s="1"/>
     </row>
-    <row r="31" spans="1:10" ht="18" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:10" ht="18" x14ac:dyDescent="0.4">
       <c r="A31" s="47"/>
       <c r="B31" s="21" t="s">
         <v>19</v>
       </c>
       <c r="C31" s="21"/>
-      <c r="D31" s="58"/>
+      <c r="D31" s="73"/>
       <c r="E31" s="1"/>
       <c r="F31" s="1"/>
       <c r="G31" s="1"/>
       <c r="H31" s="1"/>
     </row>
-    <row r="32" spans="1:10" ht="18" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:10" ht="17.5" x14ac:dyDescent="0.35">
       <c r="A32" s="1"/>
       <c r="B32" s="1"/>
       <c r="C32" s="1"/>
@@ -2043,17 +2046,17 @@
       <c r="G32" s="1"/>
       <c r="H32" s="1"/>
     </row>
-    <row r="35" spans="1:10" ht="18.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:10" ht="18.5" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A35" s="47" t="s">
         <v>15</v>
       </c>
-      <c r="B35" s="59">
+      <c r="B35" s="72">
         <v>2.5</v>
       </c>
-      <c r="C35" s="59"/>
-      <c r="D35" s="59"/>
-      <c r="E35" s="59"/>
-      <c r="F35" s="59"/>
+      <c r="C35" s="72"/>
+      <c r="D35" s="72"/>
+      <c r="E35" s="72"/>
+      <c r="F35" s="72"/>
       <c r="G35" s="47" t="s">
         <v>2</v>
       </c>
@@ -2063,12 +2066,12 @@
       <c r="I35" s="47" t="s">
         <v>4</v>
       </c>
-      <c r="J35" s="56">
+      <c r="J35" s="69">
         <f>B35/(B36-(D36+F36))+H35</f>
         <v>7.8312570781426949E-2</v>
       </c>
     </row>
-    <row r="36" spans="1:10" ht="18" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:10" ht="18" x14ac:dyDescent="0.4">
       <c r="A36" s="47"/>
       <c r="B36" s="21">
         <v>90</v>
@@ -2088,31 +2091,19 @@
       <c r="G36" s="47"/>
       <c r="H36" s="47"/>
       <c r="I36" s="47"/>
-      <c r="J36" s="56"/>
+      <c r="J36" s="69"/>
     </row>
   </sheetData>
   <mergeCells count="39">
-    <mergeCell ref="A2:F2"/>
-    <mergeCell ref="A4:A7"/>
-    <mergeCell ref="B4:B5"/>
-    <mergeCell ref="C4:C5"/>
-    <mergeCell ref="E4:E7"/>
-    <mergeCell ref="F4:F7"/>
-    <mergeCell ref="B6:D6"/>
-    <mergeCell ref="B7:D7"/>
-    <mergeCell ref="A10:A13"/>
-    <mergeCell ref="B10:B11"/>
-    <mergeCell ref="G10:G12"/>
-    <mergeCell ref="H10:H11"/>
-    <mergeCell ref="I10:I12"/>
-    <mergeCell ref="K10:K13"/>
-    <mergeCell ref="L10:L13"/>
-    <mergeCell ref="M10:M13"/>
-    <mergeCell ref="N10:N13"/>
-    <mergeCell ref="D11:F11"/>
-    <mergeCell ref="B12:D12"/>
-    <mergeCell ref="B13:F13"/>
-    <mergeCell ref="J10:J13"/>
+    <mergeCell ref="I35:I36"/>
+    <mergeCell ref="J35:J36"/>
+    <mergeCell ref="B28:H28"/>
+    <mergeCell ref="A30:A31"/>
+    <mergeCell ref="D30:D31"/>
+    <mergeCell ref="A35:A36"/>
+    <mergeCell ref="B35:F35"/>
+    <mergeCell ref="G35:G36"/>
+    <mergeCell ref="H35:H36"/>
     <mergeCell ref="A16:J16"/>
     <mergeCell ref="A18:J18"/>
     <mergeCell ref="A20:J20"/>
@@ -2122,17 +2113,41 @@
     <mergeCell ref="G25:G26"/>
     <mergeCell ref="H25:H26"/>
     <mergeCell ref="B26:F26"/>
-    <mergeCell ref="I35:I36"/>
-    <mergeCell ref="J35:J36"/>
-    <mergeCell ref="B28:H28"/>
-    <mergeCell ref="A30:A31"/>
-    <mergeCell ref="D30:D31"/>
-    <mergeCell ref="A35:A36"/>
-    <mergeCell ref="B35:F35"/>
-    <mergeCell ref="G35:G36"/>
-    <mergeCell ref="H35:H36"/>
+    <mergeCell ref="K10:K13"/>
+    <mergeCell ref="L10:L13"/>
+    <mergeCell ref="M10:M13"/>
+    <mergeCell ref="N10:N13"/>
+    <mergeCell ref="D11:F11"/>
+    <mergeCell ref="B12:D12"/>
+    <mergeCell ref="B13:F13"/>
+    <mergeCell ref="J10:J13"/>
+    <mergeCell ref="A10:A13"/>
+    <mergeCell ref="B10:B11"/>
+    <mergeCell ref="G10:G12"/>
+    <mergeCell ref="H10:H11"/>
+    <mergeCell ref="I10:I12"/>
+    <mergeCell ref="A2:F2"/>
+    <mergeCell ref="A4:A7"/>
+    <mergeCell ref="B4:B5"/>
+    <mergeCell ref="C4:C5"/>
+    <mergeCell ref="E4:E7"/>
+    <mergeCell ref="F4:F7"/>
+    <mergeCell ref="B6:D6"/>
+    <mergeCell ref="B7:D7"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{19272D62-DB20-44C8-8638-59F2608CEA8F}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>